<commit_message>
Added YPR analysis function
</commit_message>
<xml_diff>
--- a/Kaupulehu/Species_List.xlsx
+++ b/Kaupulehu/Species_List.xlsx
@@ -1,26 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eristig/Desktop/TNC/LBSPR_Kaupulehu/Kaupulehu/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud\TNC\Hawaii\SizeLimit\R code\LBSPR\Kaupulehu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01416F21-5104-2F48-BFE9-061F8F9B7D55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114EB411-B155-43A0-8F23-D0760618BA14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Species_List" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="96">
   <si>
     <t>Family</t>
   </si>
@@ -121,9 +131,6 @@
     <t>Naso hexacanthus</t>
   </si>
   <si>
-    <t>‘_pelu kala</t>
-  </si>
-  <si>
     <t>16in</t>
   </si>
   <si>
@@ -305,13 +312,19 @@
   </si>
   <si>
     <t>LINF_TL (mm)</t>
+  </si>
+  <si>
+    <t>kala lolo</t>
+  </si>
+  <si>
+    <t>Opelu kala</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1154,13 +1167,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AB33" sqref="AB33"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="14.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1180,10 +1193,10 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
@@ -1225,31 +1238,31 @@
         <v>18</v>
       </c>
       <c r="V1" t="s">
+        <v>84</v>
+      </c>
+      <c r="W1" t="s">
         <v>85</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>86</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>87</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>88</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>89</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>90</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>91</v>
       </c>
-      <c r="AC1" t="s">
-        <v>92</v>
-      </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1324,7 +1337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1399,7 +1412,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1474,7 +1487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1552,7 +1565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:29" s="1" customFormat="1">
+    <row r="6" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1593,14 +1606,11 @@
       <c r="P6" s="1">
         <v>3.2429700000000001</v>
       </c>
-      <c r="R6" s="1" t="s">
-        <v>28</v>
+      <c r="R6" t="s">
+        <v>94</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>31</v>
@@ -1622,12 +1632,12 @@
         <v>0.63880504659203563</v>
       </c>
       <c r="Z6" s="1">
-        <f>14*25.4</f>
-        <v>355.59999999999997</v>
+        <f>W6</f>
+        <v>269</v>
       </c>
       <c r="AA6">
-        <f t="shared" si="6"/>
-        <v>356.59999999999997</v>
+        <f>X6</f>
+        <v>270</v>
       </c>
       <c r="AB6">
         <v>0.4</v>
@@ -1636,7 +1646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="1" customFormat="1">
+    <row r="7" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1678,13 +1688,13 @@
         <v>2.8540000000000001</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>31</v>
@@ -1720,12 +1730,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1765,7 +1775,7 @@
         <v>25</v>
       </c>
       <c r="R8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="V8">
         <f t="shared" si="1"/>
@@ -1798,12 +1808,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:29" s="1" customFormat="1">
+    <row r="9" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -1882,12 +1892,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:29" s="1" customFormat="1">
+    <row r="10" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="1">
         <v>180</v>
@@ -1918,10 +1928,10 @@
         <v>25</v>
       </c>
       <c r="R10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="V10">
         <f t="shared" si="1"/>
@@ -1954,12 +1964,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:29" s="1" customFormat="1">
+    <row r="11" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E11" s="1">
         <v>0.87</v>
@@ -1996,16 +2006,16 @@
         <v>2.9129999999999998</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U11" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="V11">
         <f t="shared" si="1"/>
@@ -2038,12 +2048,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:29" s="1" customFormat="1">
+    <row r="12" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1">
         <v>0.94</v>
@@ -2080,16 +2090,16 @@
         <v>3.0009999999999999</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U12" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="V12">
         <f t="shared" si="1"/>
@@ -2122,12 +2132,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:29" s="1" customFormat="1">
+    <row r="13" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="1">
         <v>0.84</v>
@@ -2164,16 +2174,16 @@
         <v>2.9409999999999998</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U13" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="V13">
         <f t="shared" si="1"/>
@@ -2206,12 +2216,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:29" s="1" customFormat="1">
+    <row r="14" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1">
         <v>0.9</v>
@@ -2251,16 +2261,16 @@
         <v>2.9860000000000002</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S14" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U14" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="U14" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="V14">
         <f t="shared" si="1"/>
@@ -2293,12 +2303,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15">
         <v>0.84</v>
@@ -2365,12 +2375,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16">
         <v>0.9</v>
@@ -2434,12 +2444,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G17">
         <v>1272</v>
@@ -2497,12 +2507,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
         <v>52</v>
-      </c>
-      <c r="B18" t="s">
-        <v>53</v>
       </c>
       <c r="E18">
         <v>0.78</v>
@@ -2566,12 +2576,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
         <v>54</v>
-      </c>
-      <c r="B19" t="s">
-        <v>55</v>
       </c>
       <c r="C19">
         <v>0.92</v>
@@ -2638,12 +2648,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G20">
         <v>340</v>
@@ -2701,12 +2711,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:29" s="1" customFormat="1">
+    <row r="21" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="G21" s="1">
         <v>609</v>
@@ -2734,13 +2744,13 @@
         <v>3.089</v>
       </c>
       <c r="R21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="S21" s="1" t="s">
+      <c r="T21" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="U21" s="1" t="s">
         <v>31</v>
@@ -2776,12 +2786,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:29" s="1" customFormat="1">
+    <row r="22" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="C22" s="1">
         <v>0.92</v>
@@ -2818,16 +2828,16 @@
         <v>3.21</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U22" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="U22" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="V22">
         <f t="shared" si="1"/>
@@ -2860,12 +2870,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23">
         <v>0.85</v>
@@ -2932,12 +2942,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:29" s="1" customFormat="1">
+    <row r="24" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="1">
         <v>0.9</v>
@@ -2974,13 +2984,13 @@
         <v>3.21082</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S24" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U24" s="1" t="s">
         <v>31</v>
@@ -3016,12 +3026,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:29" s="1" customFormat="1">
+    <row r="25" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" s="1">
         <v>0.9</v>
@@ -3058,13 +3068,13 @@
         <v>3.21082</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S25" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U25" s="1" t="s">
         <v>31</v>
@@ -3100,12 +3110,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:29">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
         <v>74</v>
-      </c>
-      <c r="B26" t="s">
-        <v>75</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3175,12 +3185,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:29" s="1" customFormat="1">
+    <row r="27" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C27" s="1">
         <v>0.97</v>
@@ -3220,13 +3230,13 @@
         <v>3.3187099999999998</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S27" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U27" s="1" t="s">
         <v>31</v>
@@ -3262,12 +3272,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:29" s="1" customFormat="1">
+    <row r="28" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C28" s="1">
         <v>0.91</v>
@@ -3304,13 +3314,13 @@
         <v>3.109</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="T28" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U28" s="1" t="s">
         <v>31</v>
@@ -3346,12 +3356,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:29" s="1" customFormat="1">
+    <row r="29" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="E29" s="1">
         <v>0.82</v>
@@ -3385,7 +3395,7 @@
         <v>2.99</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V29">
         <f t="shared" si="1"/>
@@ -3414,12 +3424,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
         <v>83</v>
-      </c>
-      <c r="B30" t="s">
-        <v>84</v>
       </c>
       <c r="C30">
         <v>0.89</v>

</xml_diff>